<commit_message>
2025-07-10 Added Kanji Images for n2
</commit_message>
<xml_diff>
--- a/public/docs/kanji_n2.xlsx
+++ b/public/docs/kanji_n2.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="83">
   <si>
     <t>Kanji</t>
   </si>
@@ -30,172 +30,291 @@
     <t>English</t>
   </si>
   <si>
+    <t>てい</t>
+  </si>
+  <si>
+    <t>げん</t>
+  </si>
+  <si>
+    <t>あた.える</t>
+  </si>
+  <si>
+    <t>きょう</t>
+  </si>
+  <si>
+    <t>あつ</t>
+  </si>
+  <si>
+    <t>はん</t>
+  </si>
+  <si>
+    <t>にん</t>
+  </si>
+  <si>
+    <t>び</t>
+  </si>
+  <si>
+    <t>こう</t>
+  </si>
+  <si>
+    <t>かく</t>
+  </si>
+  <si>
+    <t>せき</t>
+  </si>
+  <si>
+    <t>しめ.す</t>
+  </si>
+  <si>
+    <t>かい</t>
+  </si>
+  <si>
+    <t>だん</t>
+  </si>
+  <si>
+    <t>たい</t>
+  </si>
+  <si>
+    <t>ひょう</t>
+  </si>
+  <si>
+    <t>propose</t>
+  </si>
+  <si>
+    <t>increase</t>
+  </si>
+  <si>
+    <t>decrease</t>
+  </si>
+  <si>
+    <t>give</t>
+  </si>
+  <si>
+    <t>situation</t>
+  </si>
+  <si>
+    <t>pressure</t>
+  </si>
+  <si>
+    <t>judge</t>
+  </si>
+  <si>
+    <t>recognize</t>
+  </si>
+  <si>
+    <t>prepare</t>
+  </si>
+  <si>
+    <t>limit</t>
+  </si>
+  <si>
+    <t>construct</t>
+  </si>
+  <si>
+    <t>confirm</t>
+  </si>
+  <si>
+    <t>responsibility</t>
+  </si>
+  <si>
+    <t>achievement</t>
+  </si>
+  <si>
+    <t>show</t>
+  </si>
+  <si>
+    <t>solve</t>
+  </si>
+  <si>
+    <t>decide</t>
+  </si>
+  <si>
+    <t>condition</t>
+  </si>
+  <si>
+    <t>evaluate</t>
+  </si>
+  <si>
+    <t>ImageName</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
     <t>提</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>n2_purpose.webp</t>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>増</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>n2_increase.jpeg</t>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>減</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>n2_decrease.webp</t>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>与</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>n2_give.jpg</t>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>況</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>n2_situation.jpg</t>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>圧</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>n2_pressure.webp</t>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>判</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>n2_judge.webp</t>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>認</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>n2_recognize.jpg</t>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>備</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>n2_prepare.jpg</t>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>限</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>n2_limit.jpg</t>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>構</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>n2_construct.jpg</t>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>確</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>n2_confirm.png</t>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>責</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>n2_responsibility.webp</t>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>績</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>n2_achievements.png</t>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>示</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>n2_show.jpg</t>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>解</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>n2_solve.jpg</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ふえる</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>へる</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>増減</t>
+    <rPh sb="0" eb="2">
+      <t>ゾウゲン</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ぞうげん</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>increase/decrease</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>n2_increase_decrease.webp</t>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>断</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>n2_decide.jpg</t>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>態</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>n2_condition.jpg</t>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>評</t>
-  </si>
-  <si>
-    <t>てい</t>
-  </si>
-  <si>
-    <t>ぞう</t>
-  </si>
-  <si>
-    <t>げん</t>
-  </si>
-  <si>
-    <t>あた.える</t>
-  </si>
-  <si>
-    <t>きょう</t>
-  </si>
-  <si>
-    <t>あつ</t>
-  </si>
-  <si>
-    <t>はん</t>
-  </si>
-  <si>
-    <t>にん</t>
-  </si>
-  <si>
-    <t>び</t>
-  </si>
-  <si>
-    <t>こう</t>
-  </si>
-  <si>
-    <t>かく</t>
-  </si>
-  <si>
-    <t>せき</t>
-  </si>
-  <si>
-    <t>しめ.す</t>
-  </si>
-  <si>
-    <t>かい</t>
-  </si>
-  <si>
-    <t>だん</t>
-  </si>
-  <si>
-    <t>たい</t>
-  </si>
-  <si>
-    <t>ひょう</t>
-  </si>
-  <si>
-    <t>propose</t>
-  </si>
-  <si>
-    <t>increase</t>
-  </si>
-  <si>
-    <t>decrease</t>
-  </si>
-  <si>
-    <t>give</t>
-  </si>
-  <si>
-    <t>situation</t>
-  </si>
-  <si>
-    <t>pressure</t>
-  </si>
-  <si>
-    <t>judge</t>
-  </si>
-  <si>
-    <t>recognize</t>
-  </si>
-  <si>
-    <t>prepare</t>
-  </si>
-  <si>
-    <t>limit</t>
-  </si>
-  <si>
-    <t>construct</t>
-  </si>
-  <si>
-    <t>confirm</t>
-  </si>
-  <si>
-    <t>responsibility</t>
-  </si>
-  <si>
-    <t>achievement</t>
-  </si>
-  <si>
-    <t>show</t>
-  </si>
-  <si>
-    <t>solve</t>
-  </si>
-  <si>
-    <t>decide</t>
-  </si>
-  <si>
-    <t>condition</t>
-  </si>
-  <si>
-    <t>evaluate</t>
-  </si>
-  <si>
-    <t>ImageName</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>n2_evaluate.png</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -574,7 +693,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -590,231 +709,292 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>22</v>
-      </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>41</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>72</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>73</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>74</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>75</v>
+      </c>
+      <c r="D5" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>43</v>
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>47</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>45</v>
+        <v>24</v>
+      </c>
+      <c r="D8" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
+        <v>25</v>
+      </c>
+      <c r="D9" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>47</v>
+        <v>26</v>
+      </c>
+      <c r="D10" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>55</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>48</v>
+        <v>27</v>
+      </c>
+      <c r="D11" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>49</v>
+        <v>28</v>
+      </c>
+      <c r="D12" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>59</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>29</v>
+      </c>
+      <c r="D13" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>51</v>
+        <v>30</v>
+      </c>
+      <c r="D14" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>63</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>52</v>
+        <v>31</v>
+      </c>
+      <c r="D15" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>77</v>
+      </c>
+      <c r="B19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>79</v>
+      </c>
+      <c r="B20" t="s">
         <v>17</v>
       </c>
-      <c r="B16" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="C20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>81</v>
+      </c>
+      <c r="B21" t="s">
         <v>18</v>
       </c>
-      <c r="B17" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" t="s">
+      <c r="C21" t="s">
         <v>37</v>
       </c>
-      <c r="C20" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" t="s">
-        <v>38</v>
-      </c>
-      <c r="C21" t="s">
-        <v>57</v>
+      <c r="D21" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>